<commit_message>
XLXS file has been corrected
</commit_message>
<xml_diff>
--- a/Basura DB.xlsx
+++ b/Basura DB.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ITESO\Diseño de Software\Repositorios\StreamingDS-JO-VC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13AFE35-1755-41F8-AAE4-E3FC37130D00}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1590" yWindow="4230" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -670,21 +679,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -694,7 +703,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -704,67 +713,43 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="9439275" cy="5915025"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -954,25 +939,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.43"/>
-    <col customWidth="1" min="2" max="2" width="35.14"/>
-    <col customWidth="1" min="5" max="5" width="18.43"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -989,9 +977,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -1006,9 +994,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
@@ -1023,9 +1011,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -1040,9 +1028,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>13</v>
@@ -1057,9 +1045,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>14</v>
@@ -1074,9 +1062,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>16</v>
@@ -1091,9 +1079,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>17</v>
@@ -1108,9 +1096,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>18</v>
@@ -1125,9 +1113,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
@@ -1142,9 +1130,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>20</v>
@@ -1159,9 +1147,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>21</v>
@@ -1176,9 +1164,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>23</v>
@@ -1193,9 +1181,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>24</v>
@@ -1210,9 +1198,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>25</v>
@@ -1227,9 +1215,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>26</v>
@@ -1244,9 +1232,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>27</v>
@@ -1261,9 +1249,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>29</v>
@@ -1278,9 +1266,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>30</v>
@@ -1295,9 +1283,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>31</v>
@@ -1312,9 +1300,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>32</v>
@@ -1329,9 +1317,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>34</v>
@@ -1346,9 +1334,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>35</v>
@@ -1363,9 +1351,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>37</v>
@@ -1380,9 +1368,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>38</v>
@@ -1397,9 +1385,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>39</v>
@@ -1414,9 +1402,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>40</v>
@@ -1431,9 +1419,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>41</v>
@@ -1448,9 +1436,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>42</v>
@@ -1465,9 +1453,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>43</v>
@@ -1482,9 +1470,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>44</v>
@@ -1499,9 +1487,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>45</v>
@@ -1516,9 +1504,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>46</v>
@@ -1533,9 +1521,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>47</v>
@@ -1550,9 +1538,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>48</v>
@@ -1567,9 +1555,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>49</v>
@@ -1584,9 +1572,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>50</v>
@@ -1601,9 +1589,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>51</v>
@@ -1618,9 +1606,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>52</v>
@@ -1635,9 +1623,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>53</v>
@@ -1652,9 +1640,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>54</v>
@@ -1669,9 +1657,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>55</v>
@@ -1686,9 +1674,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>56</v>
@@ -1703,9 +1691,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>57</v>
@@ -1720,9 +1708,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>58</v>
@@ -1737,9 +1725,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>59</v>
@@ -1754,9 +1742,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>60</v>
@@ -1771,9 +1759,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>61</v>
@@ -1788,9 +1776,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>62</v>
@@ -1805,9 +1793,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>63</v>
@@ -1822,9 +1810,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>65</v>
@@ -1839,9 +1827,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>67</v>
@@ -1856,9 +1844,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>68</v>
@@ -1873,9 +1861,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>69</v>
@@ -1890,9 +1878,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>70</v>
@@ -1907,9 +1895,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>71</v>
@@ -1924,9 +1912,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>72</v>
@@ -1941,9 +1929,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>73</v>
@@ -1958,9 +1946,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>74</v>
@@ -1975,9 +1963,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>75</v>
@@ -1992,9 +1980,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>76</v>
@@ -2009,9 +1997,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>77</v>
@@ -2026,9 +2014,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>78</v>
@@ -2043,9 +2031,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>79</v>
@@ -2060,9 +2048,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>80</v>
@@ -2077,9 +2065,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>81</v>
@@ -2094,9 +2082,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>66.0</v>
+        <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>82</v>
@@ -2111,9 +2099,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>67.0</v>
+        <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>83</v>
@@ -2128,9 +2116,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>84</v>
@@ -2145,9 +2133,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>85</v>
@@ -2162,9 +2150,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>86</v>
@@ -2179,9 +2167,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>87</v>
@@ -2196,9 +2184,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>88</v>
@@ -2213,9 +2201,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>89</v>
@@ -2230,9 +2218,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>90</v>
@@ -2247,9 +2235,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>91</v>
@@ -2264,9 +2252,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>76.0</v>
+        <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>92</v>
@@ -2281,9 +2269,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>93</v>
@@ -2298,9 +2286,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>94</v>
@@ -2315,9 +2303,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>95</v>
@@ -2332,9 +2320,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>96</v>
@@ -2349,9 +2337,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>81.0</v>
+        <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>97</v>
@@ -2366,9 +2354,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>98</v>
@@ -2383,9 +2371,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>99</v>
@@ -2400,9 +2388,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>84.0</v>
+        <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>100</v>
@@ -2417,9 +2405,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>101</v>
@@ -2434,9 +2422,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>86.0</v>
+        <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>102</v>
@@ -2451,9 +2439,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>87.0</v>
+        <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>103</v>
@@ -2468,9 +2456,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>88.0</v>
+        <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>104</v>
@@ -2485,9 +2473,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>89.0</v>
+        <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>105</v>
@@ -2502,9 +2490,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>106</v>
@@ -2519,9 +2507,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>91.0</v>
+        <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>107</v>
@@ -2536,9 +2524,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>92.0</v>
+        <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>108</v>
@@ -2553,9 +2541,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>93.0</v>
+        <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>109</v>
@@ -2570,9 +2558,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>110</v>
@@ -2587,9 +2575,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>95.0</v>
+        <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>111</v>
@@ -2604,9 +2592,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>112</v>
@@ -2621,9 +2609,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>113</v>
@@ -2638,9 +2626,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>114</v>
@@ -2655,9 +2643,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>115</v>
@@ -2672,9 +2660,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>116</v>
@@ -2689,9 +2677,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>117</v>
@@ -2706,9 +2694,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>118</v>
@@ -2723,9 +2711,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>119</v>
@@ -2740,9 +2728,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>120</v>
@@ -2757,9 +2745,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>121</v>
@@ -2774,9 +2762,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>106.0</v>
+        <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>122</v>
@@ -2791,9 +2779,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>107.0</v>
+        <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>123</v>
@@ -2808,9 +2796,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>108.0</v>
+        <v>108</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>124</v>
@@ -2825,9 +2813,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>109.0</v>
+        <v>109</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>125</v>
@@ -2842,9 +2830,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>126</v>
@@ -2859,9 +2847,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>111.0</v>
+        <v>111</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>127</v>
@@ -2876,9 +2864,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>112.0</v>
+        <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>128</v>
@@ -2893,9 +2881,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>113.0</v>
+        <v>113</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>129</v>
@@ -2910,9 +2898,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>114.0</v>
+        <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>130</v>
@@ -2927,9 +2915,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>115.0</v>
+        <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>131</v>
@@ -2944,9 +2932,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>116.0</v>
+        <v>116</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>132</v>
@@ -2961,9 +2949,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>117.0</v>
+        <v>117</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>133</v>
@@ -2978,9 +2966,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>118.0</v>
+        <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>134</v>
@@ -2995,9 +2983,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>119.0</v>
+        <v>119</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>135</v>
@@ -3012,9 +3000,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>136</v>
@@ -3029,9 +3017,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>121.0</v>
+        <v>121</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>137</v>
@@ -3046,9 +3034,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>122.0</v>
+        <v>122</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>138</v>
@@ -3063,9 +3051,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>123.0</v>
+        <v>123</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>139</v>
@@ -3080,9 +3068,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>124.0</v>
+        <v>124</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>140</v>
@@ -3097,9 +3085,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>141</v>
@@ -3114,9 +3102,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>126.0</v>
+        <v>126</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>142</v>
@@ -3131,9 +3119,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>127.0</v>
+        <v>127</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>143</v>
@@ -3148,9 +3136,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>128.0</v>
+        <v>128</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>144</v>
@@ -3165,9 +3153,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>129.0</v>
+        <v>129</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>145</v>
@@ -3182,9 +3170,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>146</v>
@@ -3199,9 +3187,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>131.0</v>
+        <v>131</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>147</v>
@@ -3216,9 +3204,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>132.0</v>
+        <v>132</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>148</v>
@@ -3233,9 +3221,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>133.0</v>
+        <v>133</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>149</v>
@@ -3250,9 +3238,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>134.0</v>
+        <v>134</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>150</v>
@@ -3267,9 +3255,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>135.0</v>
+        <v>135</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>151</v>
@@ -3284,9 +3272,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>136.0</v>
+        <v>136</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>152</v>
@@ -3301,9 +3289,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>137.0</v>
+        <v>137</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>153</v>
@@ -3318,9 +3306,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>138.0</v>
+        <v>138</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>154</v>
@@ -3335,9 +3323,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>139.0</v>
+        <v>139</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>155</v>
@@ -3352,9 +3340,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>157</v>
@@ -3369,9 +3357,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>141.0</v>
+        <v>141</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>158</v>
@@ -3386,9 +3374,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>142.0</v>
+        <v>142</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>159</v>
@@ -3403,9 +3391,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>143.0</v>
+        <v>143</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>160</v>
@@ -3420,9 +3408,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>144.0</v>
+        <v>144</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>161</v>
@@ -3437,9 +3425,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>145.0</v>
+        <v>145</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>162</v>
@@ -3454,9 +3442,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>146.0</v>
+        <v>146</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>163</v>
@@ -3471,9 +3459,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>147.0</v>
+        <v>147</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>164</v>
@@ -3488,9 +3476,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>148.0</v>
+        <v>148</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>165</v>
@@ -3505,9 +3493,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>149.0</v>
+        <v>149</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>166</v>
@@ -3522,9 +3510,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>167</v>
@@ -3539,9 +3527,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>151.0</v>
+        <v>151</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>168</v>
@@ -3556,9 +3544,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>152.0</v>
+        <v>152</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>169</v>
@@ -3573,9 +3561,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>153.0</v>
+        <v>153</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>170</v>
@@ -3590,9 +3578,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>154.0</v>
+        <v>154</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>171</v>
@@ -3607,9 +3595,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>155.0</v>
+        <v>155</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>172</v>
@@ -3624,9 +3612,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>156.0</v>
+        <v>156</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>173</v>
@@ -3641,9 +3629,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>157.0</v>
+        <v>157</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>174</v>
@@ -3658,9 +3646,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>158.0</v>
+        <v>158</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>175</v>
@@ -3675,9 +3663,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>159.0</v>
+        <v>159</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>176</v>
@@ -3692,9 +3680,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>160.0</v>
+        <v>160</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>177</v>
@@ -3709,9 +3697,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>161.0</v>
+        <v>161</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>178</v>
@@ -3726,9 +3714,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>179</v>
@@ -3743,9 +3731,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>163.0</v>
+        <v>163</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>180</v>
@@ -3760,9 +3748,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>164.0</v>
+        <v>164</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>181</v>
@@ -3777,9 +3765,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>165.0</v>
+        <v>165</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>182</v>
@@ -3794,9 +3782,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>166.0</v>
+        <v>166</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>183</v>
@@ -3811,9 +3799,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>167.0</v>
+        <v>167</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>184</v>
@@ -3828,9 +3816,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>168.0</v>
+        <v>168</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>185</v>
@@ -3845,9 +3833,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>169.0</v>
+        <v>169</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>186</v>
@@ -3862,9 +3850,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>170.0</v>
+        <v>170</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>187</v>
@@ -3879,9 +3867,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>171.0</v>
+        <v>171</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>188</v>
@@ -3896,9 +3884,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>172.0</v>
+        <v>172</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>189</v>
@@ -3913,9 +3901,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>173.0</v>
+        <v>173</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>190</v>
@@ -3930,9 +3918,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>174.0</v>
+        <v>174</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>191</v>
@@ -3947,9 +3935,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>175.0</v>
+        <v>175</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>192</v>
@@ -3964,9 +3952,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>176.0</v>
+        <v>176</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>193</v>
@@ -3981,9 +3969,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>177.0</v>
+        <v>177</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>194</v>
@@ -3998,9 +3986,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>178.0</v>
+        <v>178</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>195</v>
@@ -4015,9 +4003,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>179.0</v>
+        <v>179</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>196</v>
@@ -4032,9 +4020,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>197</v>
@@ -4049,9 +4037,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>181.0</v>
+        <v>181</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>198</v>
@@ -4066,9 +4054,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>182.0</v>
+        <v>182</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>199</v>
@@ -4083,9 +4071,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>183.0</v>
+        <v>183</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>200</v>
@@ -4100,9 +4088,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>184.0</v>
+        <v>184</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>201</v>
@@ -4117,9 +4105,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>185.0</v>
+        <v>185</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>202</v>
@@ -4134,9 +4122,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>186.0</v>
+        <v>186</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>203</v>
@@ -4151,9 +4139,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>187.0</v>
+        <v>187</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>204</v>
@@ -4168,9 +4156,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>188.0</v>
+        <v>188</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>205</v>
@@ -4185,9 +4173,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>189.0</v>
+        <v>189</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>206</v>
@@ -4202,9 +4190,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>190.0</v>
+        <v>190</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>207</v>
@@ -4219,9 +4207,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>191.0</v>
+        <v>191</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>208</v>
@@ -4236,9 +4224,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>192.0</v>
+        <v>192</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>209</v>
@@ -4253,9 +4241,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>193.0</v>
+        <v>193</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>210</v>
@@ -4270,9 +4258,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>194.0</v>
+        <v>194</v>
       </c>
       <c r="B195" s="3" t="s">
         <v>211</v>
@@ -4287,9 +4275,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>195.0</v>
+        <v>195</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>212</v>
@@ -4304,9 +4292,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>196.0</v>
+        <v>196</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>213</v>
@@ -4321,9 +4309,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>197.0</v>
+        <v>197</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>214</v>
@@ -4338,9 +4326,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>198.0</v>
+        <v>198</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>215</v>
@@ -4355,9 +4343,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>199.0</v>
+        <v>199</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>216</v>
@@ -4372,9 +4360,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>217</v>
@@ -4390,6 +4378,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>